<commit_message>
Auto stash before revert of "added send email"
</commit_message>
<xml_diff>
--- a/metadata/error-codes.xlsx
+++ b/metadata/error-codes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokke\Documents\knowbi-pentaho-error-handling-framework-brulok\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shila\Documents\Github\knowbi-pentaho-error-handling-framework\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171C6FB9-6796-4CBF-BE54-BED26F64B545}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptions" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>syscode</t>
   </si>
@@ -225,12 +226,30 @@
   </si>
   <si>
     <t>Error %SYSTEM%</t>
+  </si>
+  <si>
+    <t>Error %SYSTEM%, %SUBSYSTEM%, %LEVEL%</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>010201</t>
+  </si>
+  <si>
+    <t>010301</t>
+  </si>
+  <si>
+    <t>010401</t>
+  </si>
+  <si>
+    <t>010501</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="000000"/>
@@ -656,22 +675,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="95.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="95.33203125" customWidth="1"/>
+    <col min="8" max="1025" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -717,7 +736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -740,7 +759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -763,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -786,7 +805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -809,7 +828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -827,7 +846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -845,7 +864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="C9" s="2"/>
       <c r="E9" s="2">
@@ -869,21 +888,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
-    <col min="3" max="1025" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="1025" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -901,7 +920,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>10101</v>
       </c>
@@ -909,16 +928,16 @@
         <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>20202</v>
       </c>
@@ -935,7 +954,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>30303</v>
       </c>
@@ -943,15 +962,83 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>10201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>10301</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>10401</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>10501</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C2:E4">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C2:E4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -960,25 +1047,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="F5:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>58</v>
       </c>
@@ -998,7 +1085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1021,7 +1108,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1029,13 +1116,93 @@
         <v>20202</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
         <v>30303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1045,20 +1212,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>42</v>
       </c>
@@ -1066,7 +1233,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1074,7 +1241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1082,7 +1249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1090,7 +1257,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>

</xml_diff>